<commit_message>
Change formatting of some CFs
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_OzoneDepletion_StratosphericO3Concentration.xlsx
+++ b/src/aesa_pbs/data/aesa_OzoneDepletion_StratosphericO3Concentration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6615330E-3166-4510-9631-E86E190438D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF00E96-2E4D-4AF2-B43D-B5F61CF67605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22275" yWindow="-2280" windowWidth="11070" windowHeight="5730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +424,7 @@
   <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,7 +947,7 @@
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>1.15E-7</v>
       </c>
     </row>
@@ -957,7 +958,7 @@
       <c r="B48" t="s">
         <v>19</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>1.15E-7</v>
       </c>
     </row>
@@ -968,7 +969,7 @@
       <c r="B49" t="s">
         <v>20</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>1.15E-7</v>
       </c>
     </row>
@@ -979,7 +980,7 @@
       <c r="B50" t="s">
         <v>21</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>1.15E-7</v>
       </c>
     </row>
@@ -990,7 +991,7 @@
       <c r="B51" t="s">
         <v>22</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>1.15E-7</v>
       </c>
     </row>

</xml_diff>